<commit_message>
shortname longname staging template update for Organization
</commit_message>
<xml_diff>
--- a/StagingTemplates/Staging.Organization.xlsx
+++ b/StagingTemplates/Staging.Organization.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Aphelion\Clients\Aphelion\Meerkat\generate staging templates macro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\Meerkat\StagingTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="12420"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="28800" windowHeight="12420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>For internal use only. Do not fill in or change</t>
   </si>
@@ -41,10 +41,13 @@
     <t>Code</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>ParentOrganization_ID</t>
+  </si>
+  <si>
+    <t>ShortName</t>
+  </si>
+  <si>
+    <t>LongName</t>
   </si>
 </sst>
 </file>
@@ -373,21 +376,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet32"/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -401,10 +412,13 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>